<commit_message>
updating new coding and solution of problem.
</commit_message>
<xml_diff>
--- a/interview-assignment/sample questions.xlsx
+++ b/interview-assignment/sample questions.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koushik0004\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kousadhu\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="468" windowWidth="33600" windowHeight="19548" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9630" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -238,7 +238,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Mangal"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -246,7 +246,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Mangal"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -254,7 +254,7 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="Mangal"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -262,14 +262,14 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Mangal"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Mangal"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -496,15 +496,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="107" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="108">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -953,17 +953,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="35.4" x14ac:dyDescent="1.1499999999999999"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="99" style="2" customWidth="1"/>
     <col min="2" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="1.1499999999999999">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>55</v>
       </c>
@@ -972,7 +972,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -981,7 +981,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
@@ -990,7 +990,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="70.8" x14ac:dyDescent="1.1499999999999999">
+    <row r="4" spans="1:4" ht="42" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
@@ -999,7 +999,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="70.8" x14ac:dyDescent="1.1499999999999999">
+    <row r="5" spans="1:4" ht="42" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>3</v>
       </c>
@@ -1008,34 +1008,34 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="1.1499999999999999">
-      <c r="A6" s="19" t="s">
+    <row r="6" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="1.1499999999999999">
-      <c r="A7" s="19" t="s">
+      <c r="B6" s="18"/>
+      <c r="C6" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="1.1499999999999999">
-      <c r="A8" s="19" t="s">
+      <c r="B7" s="18"/>
+      <c r="C7" s="18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="1.1499999999999999">
+      <c r="B8" s="18"/>
+      <c r="C8" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>7</v>
       </c>
@@ -1044,16 +1044,16 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="1.1499999999999999">
-      <c r="A10" s="19" t="s">
+    <row r="10" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="70.8" x14ac:dyDescent="1.1499999999999999">
+      <c r="B10" s="18"/>
+      <c r="C10" s="18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="42" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
         <v>9</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="6" customFormat="1" ht="70.8" x14ac:dyDescent="1.1499999999999999">
+    <row r="12" spans="1:4" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
@@ -1074,7 +1074,7 @@
       </c>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" s="6" customFormat="1" ht="70.8" x14ac:dyDescent="1.1499999999999999">
+    <row r="13" spans="1:4" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1083,7 +1083,7 @@
       </c>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" s="3" customFormat="1" ht="70.8" x14ac:dyDescent="1.1499999999999999">
+    <row r="14" spans="1:4" s="3" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>15</v>
       </c>
@@ -1091,11 +1091,11 @@
       <c r="C14" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="19" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="15" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>16</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="1.1499999999999999">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
         <v>17</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="17" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>18</v>
       </c>
@@ -1122,16 +1122,16 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="1.1499999999999999">
-      <c r="A18" s="12" t="s">
+    <row r="18" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="70.8" x14ac:dyDescent="1.1499999999999999">
+      <c r="B18" s="18"/>
+      <c r="C18" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="42" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
         <v>20</v>
       </c>
@@ -1140,7 +1140,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="1.1499999999999999">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
         <v>21</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="106.2" x14ac:dyDescent="1.1499999999999999">
+    <row r="21" spans="1:3" ht="63" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
         <v>46</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="1.1499999999999999">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
         <v>22</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="3" customFormat="1" ht="283.2" x14ac:dyDescent="1.1499999999999999">
+    <row r="23" spans="1:3" s="3" customFormat="1" ht="168" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>23</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="1.1499999999999999">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
         <v>24</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="1.1499999999999999">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
         <v>25</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="70.8" x14ac:dyDescent="1.1499999999999999">
+    <row r="26" spans="1:3" ht="42" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
         <v>26</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="1.1499999999999999">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
         <v>27</v>
       </c>
@@ -1212,7 +1212,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="106.2" x14ac:dyDescent="1.1499999999999999">
+    <row r="28" spans="1:3" ht="63" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
         <v>28</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="1.1499999999999999">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
         <v>29</v>
       </c>
@@ -1230,7 +1230,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="70.8" x14ac:dyDescent="1.1499999999999999">
+    <row r="30" spans="1:3" ht="42" x14ac:dyDescent="0.35">
       <c r="A30" s="12" t="s">
         <v>30</v>
       </c>
@@ -1239,7 +1239,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="70.8" x14ac:dyDescent="1.1499999999999999">
+    <row r="31" spans="1:3" ht="42" x14ac:dyDescent="0.35">
       <c r="A31" s="12" t="s">
         <v>31</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="1.1499999999999999">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="12" t="s">
         <v>32</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="1.1499999999999999">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="12" t="s">
         <v>33</v>
       </c>
@@ -1266,16 +1266,16 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="70.8" x14ac:dyDescent="1.1499999999999999">
-      <c r="A34" s="12" t="s">
+    <row r="34" spans="1:3" s="16" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+      <c r="A34" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="177" x14ac:dyDescent="1.1499999999999999">
+      <c r="B34" s="18"/>
+      <c r="C34" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="105" x14ac:dyDescent="0.35">
       <c r="A35" s="12" t="s">
         <v>49</v>
       </c>
@@ -1284,16 +1284,16 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="141.6" x14ac:dyDescent="1.1499999999999999">
-      <c r="A36" s="12" t="s">
+    <row r="36" spans="1:3" s="16" customFormat="1" ht="63" x14ac:dyDescent="0.35">
+      <c r="A36" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="70.8" x14ac:dyDescent="1.1499999999999999">
+      <c r="B36" s="18"/>
+      <c r="C36" s="18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="42" x14ac:dyDescent="0.35">
       <c r="A37" s="12" t="s">
         <v>34</v>
       </c>
@@ -1302,30 +1302,30 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="70.8" x14ac:dyDescent="1.1499999999999999">
-      <c r="A38" s="17" t="s">
+    <row r="38" spans="1:3" s="16" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+      <c r="A38" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="1.1499999999999999">
+      <c r="B38" s="21"/>
+      <c r="C38" s="21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="12"/>
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="1.1499999999999999">
-      <c r="A40" s="12" t="s">
+    <row r="40" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="70.8" x14ac:dyDescent="1.1499999999999999">
+      <c r="B40" s="18"/>
+      <c r="C40" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="42" x14ac:dyDescent="0.35">
       <c r="A41" s="12" t="s">
         <v>36</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="106.2" x14ac:dyDescent="1.1499999999999999">
+    <row r="42" spans="1:3" ht="42" x14ac:dyDescent="0.35">
       <c r="A42" s="12" t="s">
         <v>37</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="409.6" x14ac:dyDescent="1.1499999999999999">
+    <row r="43" spans="1:3" ht="315" x14ac:dyDescent="0.35">
       <c r="A43" s="12" t="s">
         <v>52</v>
       </c>
@@ -1352,34 +1352,34 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="1.1499999999999999">
-      <c r="A44" s="12" t="s">
+    <row r="44" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B44" s="13"/>
-      <c r="C44" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="177" x14ac:dyDescent="1.1499999999999999">
-      <c r="A45" s="12" t="s">
+      <c r="B44" s="18"/>
+      <c r="C44" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" s="16" customFormat="1" ht="105" x14ac:dyDescent="0.35">
+      <c r="A45" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="B45" s="13"/>
-      <c r="C45" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="70.8" x14ac:dyDescent="1.1499999999999999">
-      <c r="A46" s="12" t="s">
+      <c r="B45" s="18"/>
+      <c r="C45" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" s="16" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+      <c r="A46" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B46" s="13"/>
-      <c r="C46" s="13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="1.1499999999999999">
+      <c r="B46" s="18"/>
+      <c r="C46" s="18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="12" t="s">
         <v>40</v>
       </c>
@@ -1388,25 +1388,25 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="1.1499999999999999">
-      <c r="A48" s="12" t="s">
+    <row r="48" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B48" s="13"/>
-      <c r="C48" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="1.1499999999999999">
-      <c r="A49" s="12" t="s">
+      <c r="B48" s="18"/>
+      <c r="C48" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B49" s="13"/>
-      <c r="C49" s="13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="1.1499999999999999">
+      <c r="B49" s="18"/>
+      <c r="C49" s="18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="12" t="s">
         <v>54</v>
       </c>
@@ -1415,16 +1415,16 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="1.1499999999999999">
-      <c r="A51" s="12" t="s">
+    <row r="51" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B51" s="13"/>
-      <c r="C51" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="1.1499999999999999">
+      <c r="B51" s="18"/>
+      <c r="C51" s="18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="12" t="s">
         <v>44</v>
       </c>
@@ -1433,12 +1433,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:3" s="16" customFormat="1" ht="177" x14ac:dyDescent="1.1499999999999999">
-      <c r="A53" s="19" t="s">
+    <row r="53" spans="1:3" s="16" customFormat="1" ht="105" x14ac:dyDescent="0.35">
+      <c r="A53" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B53" s="20"/>
-      <c r="C53" s="20" t="s">
+      <c r="B53" s="18"/>
+      <c r="C53" s="18" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
more added js logics
</commit_message>
<xml_diff>
--- a/interview-assignment/sample questions.xlsx
+++ b/interview-assignment/sample questions.xlsx
@@ -954,7 +954,7 @@
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -1406,12 +1406,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A50" s="12" t="s">
+    <row r="50" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="B50" s="13"/>
-      <c r="C50" s="13" t="s">
+      <c r="B50" s="18"/>
+      <c r="C50" s="18" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
few more coding added.
</commit_message>
<xml_diff>
--- a/interview-assignment/sample questions.xlsx
+++ b/interview-assignment/sample questions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kousadhu\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\drive-d\applications\gs-coderpad\interview-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -953,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -990,12 +990,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="42" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
+    <row r="4" spans="1:4" s="16" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+      <c r="A4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13" t="s">
+      <c r="B4" s="18"/>
+      <c r="C4" s="18" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1343,12 +1343,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="315" x14ac:dyDescent="0.35">
-      <c r="A43" s="12" t="s">
+    <row r="43" spans="1:3" s="16" customFormat="1" ht="315" x14ac:dyDescent="0.35">
+      <c r="A43" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="B43" s="13"/>
-      <c r="C43" s="13" t="s">
+      <c r="B43" s="18"/>
+      <c r="C43" s="18" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating one more coding
</commit_message>
<xml_diff>
--- a/interview-assignment/sample questions.xlsx
+++ b/interview-assignment/sample questions.xlsx
@@ -274,7 +274,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -290,12 +290,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -466,14 +460,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -483,10 +476,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -495,16 +484,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="107" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="108">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -954,7 +943,7 @@
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -964,481 +953,481 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="10" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="16" customFormat="1" ht="42" x14ac:dyDescent="0.35">
-      <c r="A4" s="17" t="s">
+      <c r="B3" s="15"/>
+      <c r="C3" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="13" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+      <c r="A4" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18" t="s">
+      <c r="B4" s="15"/>
+      <c r="C4" s="15" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="42" x14ac:dyDescent="0.35">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="17" t="s">
+      <c r="B5" s="12"/>
+      <c r="C5" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="17" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="17" t="s">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="17" t="s">
+      <c r="B8" s="15"/>
+      <c r="C8" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="17" t="s">
+      <c r="B9" s="15"/>
+      <c r="C9" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="16" customFormat="1" ht="42" x14ac:dyDescent="0.35">
-      <c r="A11" s="17" t="s">
+      <c r="B10" s="15"/>
+      <c r="C10" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="13" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+      <c r="A11" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.35">
-      <c r="A12" s="5" t="s">
+      <c r="B11" s="15"/>
+      <c r="C11" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="7"/>
-    </row>
-    <row r="13" spans="1:4" s="6" customFormat="1" ht="42" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
+      <c r="C12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="7"/>
+      <c r="C13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="6"/>
     </row>
     <row r="14" spans="1:4" s="3" customFormat="1" ht="42" x14ac:dyDescent="0.35">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="19" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="16" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6" t="s">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13" t="s">
+      <c r="B16" s="10"/>
+      <c r="C16" s="10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="17" t="s">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18" t="s">
+      <c r="B18" s="15"/>
+      <c r="C18" s="15" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="42" x14ac:dyDescent="0.35">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13" t="s">
+      <c r="B19" s="10"/>
+      <c r="C19" s="10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13" t="s">
+      <c r="B20" s="10"/>
+      <c r="C20" s="10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="63" x14ac:dyDescent="0.35">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13" t="s">
+      <c r="B21" s="10"/>
+      <c r="C21" s="10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13" t="s">
+      <c r="B22" s="10"/>
+      <c r="C22" s="10" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="3" customFormat="1" ht="168" x14ac:dyDescent="0.35">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6" t="s">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13" t="s">
+      <c r="B24" s="10"/>
+      <c r="C24" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13" t="s">
+      <c r="B25" s="10"/>
+      <c r="C25" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="42" x14ac:dyDescent="0.35">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="17" t="s">
+      <c r="B26" s="10"/>
+      <c r="C26" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" s="16" customFormat="1" ht="63" x14ac:dyDescent="0.35">
-      <c r="A28" s="17" t="s">
+      <c r="B27" s="15"/>
+      <c r="C27" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.35">
+      <c r="A28" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18" t="s">
+      <c r="B28" s="15"/>
+      <c r="C28" s="15" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13" t="s">
+      <c r="B29" s="10"/>
+      <c r="C29" s="10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="42" x14ac:dyDescent="0.35">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" s="16" customFormat="1" ht="42" x14ac:dyDescent="0.35">
-      <c r="A31" s="17" t="s">
+      <c r="B30" s="10"/>
+      <c r="C30" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" s="13" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+      <c r="A31" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18" t="s">
+      <c r="B31" s="15"/>
+      <c r="C31" s="15" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="12" t="s">
+      <c r="A32" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13" t="s">
+      <c r="B32" s="10"/>
+      <c r="C32" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" s="16" customFormat="1" ht="42" x14ac:dyDescent="0.35">
-      <c r="A34" s="17" t="s">
+      <c r="B33" s="10"/>
+      <c r="C33" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="13" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+      <c r="A34" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B34" s="18"/>
-      <c r="C34" s="18" t="s">
+      <c r="B34" s="15"/>
+      <c r="C34" s="15" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="105" x14ac:dyDescent="0.35">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" s="16" customFormat="1" ht="63" x14ac:dyDescent="0.35">
-      <c r="A36" s="17" t="s">
+      <c r="B35" s="10"/>
+      <c r="C35" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.35">
+      <c r="A36" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" s="16" customFormat="1" ht="42" x14ac:dyDescent="0.35">
-      <c r="A37" s="17" t="s">
+      <c r="B36" s="15"/>
+      <c r="C36" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" s="13" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+      <c r="A37" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" s="16" customFormat="1" ht="42" x14ac:dyDescent="0.35">
-      <c r="A38" s="20" t="s">
+      <c r="B37" s="15"/>
+      <c r="C37" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" s="13" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+      <c r="A38" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="B38" s="21"/>
-      <c r="C38" s="21" t="s">
+      <c r="B38" s="18"/>
+      <c r="C38" s="18" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" s="12"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-    </row>
-    <row r="40" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="17" t="s">
+      <c r="A39" s="9"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+    </row>
+    <row r="40" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" s="16" customFormat="1" ht="42" x14ac:dyDescent="0.35">
-      <c r="A41" s="17" t="s">
+      <c r="B40" s="15"/>
+      <c r="C40" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" s="13" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+      <c r="A41" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" s="16" customFormat="1" ht="42" x14ac:dyDescent="0.35">
-      <c r="A42" s="17" t="s">
+      <c r="B41" s="15"/>
+      <c r="C41" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" s="13" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+      <c r="A42" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" s="16" customFormat="1" ht="315" x14ac:dyDescent="0.35">
-      <c r="A43" s="17" t="s">
+      <c r="B42" s="15"/>
+      <c r="C42" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" s="13" customFormat="1" ht="315" x14ac:dyDescent="0.35">
+      <c r="A43" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="B43" s="18"/>
-      <c r="C43" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="17" t="s">
+      <c r="B43" s="15"/>
+      <c r="C43" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B44" s="18"/>
-      <c r="C44" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" s="16" customFormat="1" ht="105" x14ac:dyDescent="0.35">
-      <c r="A45" s="17" t="s">
+      <c r="B44" s="15"/>
+      <c r="C44" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" s="13" customFormat="1" ht="105" x14ac:dyDescent="0.35">
+      <c r="A45" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B45" s="18"/>
-      <c r="C45" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" s="16" customFormat="1" ht="42" x14ac:dyDescent="0.35">
-      <c r="A46" s="17" t="s">
+      <c r="B45" s="15"/>
+      <c r="C45" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" s="13" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+      <c r="A46" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18" t="s">
+      <c r="B46" s="15"/>
+      <c r="C46" s="15" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" s="12" t="s">
+      <c r="A47" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B47" s="13"/>
-      <c r="C47" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="17" t="s">
+      <c r="B47" s="10"/>
+      <c r="C47" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="17" t="s">
+      <c r="B48" s="15"/>
+      <c r="C48" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="17" t="s">
+      <c r="B49" s="15"/>
+      <c r="C49" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B50" s="18"/>
-      <c r="C50" s="18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="17" t="s">
+      <c r="B50" s="15"/>
+      <c r="C50" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B51" s="18"/>
-      <c r="C51" s="18" t="s">
+      <c r="B51" s="15"/>
+      <c r="C51" s="15" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A52" s="12" t="s">
+      <c r="A52" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B52" s="13"/>
-      <c r="C52" s="13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" s="16" customFormat="1" ht="105" x14ac:dyDescent="0.35">
-      <c r="A53" s="17" t="s">
+      <c r="B52" s="10"/>
+      <c r="C52" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" s="13" customFormat="1" ht="105" x14ac:dyDescent="0.35">
+      <c r="A53" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B53" s="18"/>
-      <c r="C53" s="18" t="s">
+      <c r="B53" s="15"/>
+      <c r="C53" s="15" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated new code with recurssion matrix spiral
</commit_message>
<xml_diff>
--- a/interview-assignment/sample questions.xlsx
+++ b/interview-assignment/sample questions.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\drive-d\applications\gs-coderpad\interview-assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\node-applications\node-rest-api\interview-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9630" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9636" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -104,12 +104,6 @@
 Avg Bobby = 315,Alex= 100,Alia=-678. Result: 315</t>
   </si>
   <si>
-    <t>Given an m*n matrix, print the matrix in reverse spiral form usingrecursion.</t>
-  </si>
-  <si>
-    <t>Find the smallest subarray whose sum is equal or greater than thetarget value</t>
-  </si>
-  <si>
     <t>Given a program to reverse a string which is incorrect. Need todebug and fix it to run executing all test cases successfully</t>
   </si>
   <si>
@@ -229,6 +223,12 @@
   <si>
     <t>https://wsvincent.com/javascript-two-sum-find-all-pairs-match-target-value/</t>
   </si>
+  <si>
+    <t>Given an m*n matrix, print the matrix in reverse spiral form using recursion.</t>
+  </si>
+  <si>
+    <t>Find the smallest subarray whose sum is equal or greater than the target value</t>
+  </si>
 </sst>
 </file>
 
@@ -238,7 +238,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Mangal"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -246,7 +246,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Mangal"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -254,7 +254,7 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="Calibri"/>
+      <name val="Mangal"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -262,14 +262,14 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Mangal"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Mangal"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -942,26 +942,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="35.4" x14ac:dyDescent="1.1499999999999999"/>
   <cols>
     <col min="1" max="1" width="99" style="2" customWidth="1"/>
     <col min="2" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="1.1499999999999999">
       <c r="A1" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -970,7 +970,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
@@ -979,7 +979,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="13" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" s="13" customFormat="1" ht="70.8" x14ac:dyDescent="1.1499999999999999">
       <c r="A4" s="14" t="s">
         <v>2</v>
       </c>
@@ -988,7 +988,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="42" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="70.8" x14ac:dyDescent="1.1499999999999999">
       <c r="A5" s="11" t="s">
         <v>3</v>
       </c>
@@ -997,7 +997,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A6" s="14" t="s">
         <v>4</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A7" s="14" t="s">
         <v>5</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A8" s="14" t="s">
         <v>6</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A9" s="14" t="s">
         <v>7</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A10" s="14" t="s">
         <v>8</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="13" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" s="13" customFormat="1" ht="70.8" x14ac:dyDescent="1.1499999999999999">
       <c r="A11" s="14" t="s">
         <v>9</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="70.8" x14ac:dyDescent="1.1499999999999999">
       <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
@@ -1063,7 +1063,7 @@
       </c>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="70.8" x14ac:dyDescent="1.1499999999999999">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
@@ -1072,7 +1072,7 @@
       </c>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:4" s="3" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" s="3" customFormat="1" ht="70.8" x14ac:dyDescent="1.1499999999999999">
       <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
@@ -1081,10 +1081,10 @@
         <v>13</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
@@ -1093,7 +1093,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="1.1499999999999999">
       <c r="A16" s="9" t="s">
         <v>17</v>
       </c>
@@ -1102,7 +1102,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A18" s="14" t="s">
         <v>19</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="42" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="70.8" x14ac:dyDescent="1.1499999999999999">
       <c r="A19" s="9" t="s">
         <v>20</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="1.1499999999999999">
       <c r="A20" s="9" t="s">
         <v>21</v>
       </c>
@@ -1138,25 +1138,25 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="63" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="106.2" x14ac:dyDescent="1.1499999999999999">
       <c r="A21" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="1.1499999999999999">
       <c r="A22" s="9" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" s="3" customFormat="1" ht="168" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="3" customFormat="1" ht="283.2" x14ac:dyDescent="1.1499999999999999">
       <c r="A23" s="4" t="s">
         <v>23</v>
       </c>
@@ -1165,266 +1165,266 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="1.1499999999999999">
+      <c r="A24" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="1.1499999999999999">
       <c r="A25" s="9" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="42" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="70.8" x14ac:dyDescent="1.1499999999999999">
       <c r="A26" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A27" s="14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B27" s="15"/>
       <c r="C27" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" s="13" customFormat="1" ht="106.2" x14ac:dyDescent="1.1499999999999999">
       <c r="A28" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B28" s="15"/>
       <c r="C28" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="1.1499999999999999">
       <c r="A29" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B29" s="10"/>
       <c r="C29" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="42" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" ht="70.8" x14ac:dyDescent="1.1499999999999999">
       <c r="A30" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="13" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" s="13" customFormat="1" ht="70.8" x14ac:dyDescent="1.1499999999999999">
       <c r="A31" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B31" s="15"/>
       <c r="C31" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="1.1499999999999999">
       <c r="A32" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B32" s="10"/>
       <c r="C32" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="1.1499999999999999">
       <c r="A33" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B33" s="10"/>
       <c r="C33" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="13" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" s="13" customFormat="1" ht="70.8" x14ac:dyDescent="1.1499999999999999">
       <c r="A34" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B34" s="15"/>
       <c r="C34" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="105" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" ht="177" x14ac:dyDescent="1.1499999999999999">
       <c r="A35" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B35" s="10"/>
       <c r="C35" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" s="13" customFormat="1" ht="141.6" x14ac:dyDescent="1.1499999999999999">
       <c r="A36" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B36" s="15"/>
       <c r="C36" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="13" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" s="13" customFormat="1" ht="70.8" x14ac:dyDescent="1.1499999999999999">
       <c r="A37" s="14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B37" s="15"/>
       <c r="C37" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="13" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" s="13" customFormat="1" ht="70.8" x14ac:dyDescent="1.1499999999999999">
       <c r="A38" s="17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B38" s="18"/>
       <c r="C38" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="1.1499999999999999">
       <c r="A39" s="9"/>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
     </row>
-    <row r="40" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A40" s="14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B40" s="15"/>
       <c r="C40" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="13" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" s="13" customFormat="1" ht="70.8" x14ac:dyDescent="1.1499999999999999">
       <c r="A41" s="14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B41" s="15"/>
       <c r="C41" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="13" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" s="13" customFormat="1" ht="106.2" x14ac:dyDescent="1.1499999999999999">
       <c r="A42" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B42" s="15"/>
       <c r="C42" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="13" customFormat="1" ht="315" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" s="13" customFormat="1" ht="409.6" x14ac:dyDescent="1.1499999999999999">
       <c r="A43" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B43" s="15"/>
       <c r="C43" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A44" s="14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B44" s="15"/>
       <c r="C44" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="13" customFormat="1" ht="105" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" s="13" customFormat="1" ht="177" x14ac:dyDescent="1.1499999999999999">
       <c r="A45" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B45" s="15"/>
       <c r="C45" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:3" s="13" customFormat="1" ht="42" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" s="13" customFormat="1" ht="70.8" x14ac:dyDescent="1.1499999999999999">
       <c r="A46" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B46" s="15"/>
       <c r="C46" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="1.1499999999999999">
       <c r="A47" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A48" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B48" s="15"/>
       <c r="C48" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A49" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B49" s="15"/>
       <c r="C49" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A50" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B50" s="15"/>
       <c r="C50" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="1.1499999999999999">
       <c r="A51" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B51" s="15"/>
       <c r="C51" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="1.1499999999999999">
       <c r="A52" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B52" s="10"/>
       <c r="C52" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:3" s="13" customFormat="1" ht="105" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" s="13" customFormat="1" ht="177" x14ac:dyDescent="1.1499999999999999">
       <c r="A53" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B53" s="15"/>
       <c r="C53" s="15" t="s">

</xml_diff>

<commit_message>
added one more coding qn number 35
</commit_message>
<xml_diff>
--- a/interview-assignment/sample questions.xlsx
+++ b/interview-assignment/sample questions.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\node-applications\node-rest-api\interview-assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\drive-d\applications\gs-coderpad\interview-assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9636" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9630" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -104,9 +104,6 @@
 Avg Bobby = 315,Alex= 100,Alia=-678. Result: 315</t>
   </si>
   <si>
-    <t>Given a program to reverse a string which is incorrect. Need todebug and fix it to run executing all test cases successfully</t>
-  </si>
-  <si>
     <t>Find the dot product of two arrays - mean array1[i] * array2[i]</t>
   </si>
   <si>
@@ -229,6 +226,9 @@
   <si>
     <t>Find the smallest subarray whose sum is equal or greater than the target value</t>
   </si>
+  <si>
+    <t>Given a program to reverse a string which is incorrect. Need to debug and fix it to run executing all test cases successfully</t>
+  </si>
 </sst>
 </file>
 
@@ -238,7 +238,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Mangal"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -246,7 +246,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="Mangal"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -254,7 +254,7 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="Mangal"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -262,14 +262,14 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Mangal"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Mangal"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -942,26 +942,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="35.4" x14ac:dyDescent="1.1499999999999999"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="99" style="2" customWidth="1"/>
     <col min="2" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="1.1499999999999999">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="1.1499999999999999">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -970,7 +970,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="3" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
@@ -979,7 +979,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="13" customFormat="1" ht="70.8" x14ac:dyDescent="1.1499999999999999">
+    <row r="4" spans="1:4" s="13" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
         <v>2</v>
       </c>
@@ -988,7 +988,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="70.8" x14ac:dyDescent="1.1499999999999999">
+    <row r="5" spans="1:4" ht="42" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>3</v>
       </c>
@@ -997,7 +997,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="6" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
         <v>4</v>
       </c>
@@ -1006,7 +1006,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="7" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>5</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="8" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
         <v>6</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="9" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
         <v>7</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="10" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>8</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="13" customFormat="1" ht="70.8" x14ac:dyDescent="1.1499999999999999">
+    <row r="11" spans="1:4" s="13" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
         <v>9</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="70.8" x14ac:dyDescent="1.1499999999999999">
+    <row r="12" spans="1:4" s="5" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
@@ -1063,7 +1063,7 @@
       </c>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="70.8" x14ac:dyDescent="1.1499999999999999">
+    <row r="13" spans="1:4" s="5" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
@@ -1072,7 +1072,7 @@
       </c>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="1:4" s="3" customFormat="1" ht="70.8" x14ac:dyDescent="1.1499999999999999">
+    <row r="14" spans="1:4" s="3" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
@@ -1081,10 +1081,10 @@
         <v>13</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="1.1499999999999999">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
@@ -1093,16 +1093,16 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="1.1499999999999999">
-      <c r="A16" s="9" t="s">
+    <row r="16" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="1.1499999999999999">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="18" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="14" t="s">
         <v>19</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="70.8" x14ac:dyDescent="1.1499999999999999">
+    <row r="19" spans="1:3" ht="42" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
         <v>20</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="1.1499999999999999">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
         <v>21</v>
       </c>
@@ -1138,25 +1138,25 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="106.2" x14ac:dyDescent="1.1499999999999999">
+    <row r="21" spans="1:3" ht="63" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B21" s="10"/>
       <c r="C21" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="1.1499999999999999">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="10"/>
       <c r="C22" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" s="3" customFormat="1" ht="283.2" x14ac:dyDescent="1.1499999999999999">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" s="3" customFormat="1" ht="168" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>23</v>
       </c>
@@ -1165,266 +1165,266 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="24" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B24" s="5"/>
       <c r="C24" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="1.1499999999999999">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="70.8" x14ac:dyDescent="1.1499999999999999">
+    <row r="26" spans="1:3" ht="42" x14ac:dyDescent="0.35">
       <c r="A26" s="9" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="27" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" s="15"/>
       <c r="C27" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="13" customFormat="1" ht="106.2" x14ac:dyDescent="1.1499999999999999">
+    <row r="28" spans="1:3" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.35">
       <c r="A28" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" s="15"/>
       <c r="C28" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="1.1499999999999999">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" s="10"/>
       <c r="C29" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="70.8" x14ac:dyDescent="1.1499999999999999">
+    <row r="30" spans="1:3" ht="42" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="13" customFormat="1" ht="70.8" x14ac:dyDescent="1.1499999999999999">
+    <row r="31" spans="1:3" s="13" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A31" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" s="15"/>
       <c r="C31" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="1.1499999999999999">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" s="10"/>
       <c r="C32" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="1.1499999999999999">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B33" s="10"/>
       <c r="C33" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="13" customFormat="1" ht="70.8" x14ac:dyDescent="1.1499999999999999">
+    <row r="34" spans="1:3" s="13" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A34" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B34" s="15"/>
       <c r="C34" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="177" x14ac:dyDescent="1.1499999999999999">
-      <c r="A35" s="9" t="s">
+    <row r="35" spans="1:3" s="3" customFormat="1" ht="105" x14ac:dyDescent="0.35">
+      <c r="A35" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" s="13" customFormat="1" ht="63" x14ac:dyDescent="0.35">
+      <c r="A36" s="14" t="s">
         <v>47</v>
-      </c>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" s="13" customFormat="1" ht="141.6" x14ac:dyDescent="1.1499999999999999">
-      <c r="A36" s="14" t="s">
-        <v>48</v>
       </c>
       <c r="B36" s="15"/>
       <c r="C36" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="13" customFormat="1" ht="70.8" x14ac:dyDescent="1.1499999999999999">
+    <row r="37" spans="1:3" s="13" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A37" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B37" s="15"/>
       <c r="C37" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="13" customFormat="1" ht="70.8" x14ac:dyDescent="1.1499999999999999">
+    <row r="38" spans="1:3" s="13" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A38" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B38" s="18"/>
       <c r="C38" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="1.1499999999999999">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="9"/>
       <c r="B39" s="10"/>
       <c r="C39" s="10"/>
     </row>
-    <row r="40" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="40" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B40" s="15"/>
       <c r="C40" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="13" customFormat="1" ht="70.8" x14ac:dyDescent="1.1499999999999999">
+    <row r="41" spans="1:3" s="13" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A41" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B41" s="15"/>
       <c r="C41" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="13" customFormat="1" ht="106.2" x14ac:dyDescent="1.1499999999999999">
+    <row r="42" spans="1:3" s="13" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A42" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B42" s="15"/>
       <c r="C42" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="13" customFormat="1" ht="409.6" x14ac:dyDescent="1.1499999999999999">
+    <row r="43" spans="1:3" s="13" customFormat="1" ht="315" x14ac:dyDescent="0.35">
       <c r="A43" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B43" s="15"/>
       <c r="C43" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="44" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B44" s="15"/>
       <c r="C44" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="13" customFormat="1" ht="177" x14ac:dyDescent="1.1499999999999999">
+    <row r="45" spans="1:3" s="13" customFormat="1" ht="105" x14ac:dyDescent="0.35">
       <c r="A45" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B45" s="15"/>
       <c r="C45" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="46" spans="1:3" s="13" customFormat="1" ht="70.8" x14ac:dyDescent="1.1499999999999999">
+    <row r="46" spans="1:3" s="13" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A46" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B46" s="15"/>
       <c r="C46" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="1.1499999999999999">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="48" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B48" s="15"/>
       <c r="C48" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="49" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B49" s="15"/>
       <c r="C49" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="50" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B50" s="15"/>
       <c r="C50" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="1.1499999999999999">
+    <row r="51" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B51" s="15"/>
       <c r="C51" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="1.1499999999999999">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B52" s="10"/>
       <c r="C52" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:3" s="13" customFormat="1" ht="177" x14ac:dyDescent="1.1499999999999999">
+    <row r="53" spans="1:3" s="13" customFormat="1" ht="105" x14ac:dyDescent="0.35">
       <c r="A53" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B53" s="15"/>
       <c r="C53" s="15" t="s">

</xml_diff>